<commit_message>
added 5 scripts for cot22; added new objects
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyCOTC022-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyCOTC022-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F826A2-DAD0-4083-9651-0ED29C158053}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A027DE-5F57-42C8-B464-8242EA73B17A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -129,6 +129,23 @@
 	count(DISTINCT(samp)) as number_of_sample , 
 	count(DISTINCT(c.case_id)) as number_of_cases , 
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['COTC022'] and demo.breed in ['American Staffordshire Terrier','Mixed Breed'] and diag.primary_disease_site in ['Bone (Appendicular)']
+WITH DISTINCT f, s
+RETURN 
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS `File Format`,
+  coalesce(f.file_size, '') AS `Size`,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -500,19 +517,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.1796875" customWidth="1"/>
+    <col min="5" max="5" width="39.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -529,7 +546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -546,7 +563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -563,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -580,7 +597,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>